<commit_message>
streamline all item handles closes #36
</commit_message>
<xml_diff>
--- a/concourse.xlsx
+++ b/concourse.xlsx
@@ -40,7 +40,7 @@
     <t>concept</t>
   </si>
   <si>
-    <t>remote-work-family</t>
+    <t>remote_work_family</t>
   </si>
   <si>
     <t>Arbeiten von zu Hause erlaubt es mir, Job und Familie problemlos zu vereinbaren.</t>
@@ -55,7 +55,7 @@
     <t>Entgrenzung Arbeit und Freizeit</t>
   </si>
   <si>
-    <t>work-creativity</t>
+    <t>work_creativity</t>
   </si>
   <si>
     <t>Bei der Arbeit kann ich meiner Kreativität freien Lauf lassen.</t>
@@ -70,7 +70,7 @@
     <t>Voß 1998</t>
   </si>
   <si>
-    <t>free-time-work-time</t>
+    <t>free_time_work_time</t>
   </si>
   <si>
     <t>Die Unterscheidung von Arbeit und Freizeit ergibt wenig Sinn für mich.</t>
@@ -82,7 +82,7 @@
     <t>The distinction between work and free-time does not make a lot of sense to me.</t>
   </si>
   <si>
-    <t>meaningful-work</t>
+    <t>meaningful_work</t>
   </si>
   <si>
     <t>Die Zeit in meiner Arbeit verbringe ich mit etwas Sinnvollem.</t>
@@ -97,7 +97,7 @@
     <t>Sinnstiftung</t>
   </si>
   <si>
-    <t>remote-job-done</t>
+    <t>remote_job_done</t>
   </si>
   <si>
     <t>Entscheidend ist nicht, wann oder wo ich arbeite, sondern dass die Arbeit getan wird.</t>
@@ -112,7 +112,7 @@
     <t>Flexibilität von Ort und Zeit von Arbeit</t>
   </si>
   <si>
-    <t>self-motivation</t>
+    <t>self_motivation</t>
   </si>
   <si>
     <t>Es ist meine Verantwortung, mich zu motivieren.</t>
@@ -127,7 +127,7 @@
     <t>Sabine Skript</t>
   </si>
   <si>
-    <t>enough-staff</t>
+    <t>enough_staff</t>
   </si>
   <si>
     <t>Für das was zu tun ist, sind wir ausreichend Leute.</t>
@@ -139,7 +139,7 @@
     <t>There is enough staff to get everything done that needs to be done.</t>
   </si>
   <si>
-    <t>team-work-late</t>
+    <t>team_work_late</t>
   </si>
   <si>
     <t>Für mein Team bleibe ich abends auch mal länger.</t>
@@ -151,7 +151,7 @@
     <t>For my team, I’m happy to sometimes work late.</t>
   </si>
   <si>
-    <t>best-pressure</t>
+    <t>best_pressure</t>
   </si>
   <si>
     <t>Ich arbeite am besten unter Druck.</t>
@@ -163,7 +163,7 @@
     <t>I perform best, when I’m under pressure.</t>
   </si>
   <si>
-    <t>work-2-live</t>
+    <t>work_2_live</t>
   </si>
   <si>
     <t>Ich arbeite, um zu leben.</t>
@@ -175,7 +175,7 @@
     <t>I work to make a living.</t>
   </si>
   <si>
-    <t>work-life-struggle</t>
+    <t>work_life_struggle</t>
   </si>
   <si>
     <t>Ich bin manchmal zerissen zwischen dem, was ich privat will und dem, was ich beruflich sollte.</t>
@@ -190,7 +190,7 @@
     <t>Klassenkampf im Herzen</t>
   </si>
   <si>
-    <t>own-boss</t>
+    <t>own_boss</t>
   </si>
   <si>
     <t>Ich bin mein eigener Chef.</t>
@@ -202,7 +202,7 @@
     <t>I am my own boss.</t>
   </si>
   <si>
-    <t>sleep-well</t>
+    <t>sleep_well</t>
   </si>
   <si>
     <t>Ich kann Aufgaben beruhigt liegen lassen, ohne schlecht zu schlafen.</t>
@@ -214,7 +214,7 @@
     <t>I can sleep well, even when there are things left undone at work.</t>
   </si>
   <si>
-    <t>live-2-work</t>
+    <t>live_2_work</t>
   </si>
   <si>
     <t>Ich lebe, um zu arbeiten.</t>
@@ -226,7 +226,7 @@
     <t>I live to work.</t>
   </si>
   <si>
-    <t>give-best</t>
+    <t>give_best</t>
   </si>
   <si>
     <t>Ich motiviere mich immer wieder das Beste zu geben.</t>
@@ -241,7 +241,7 @@
     <t>Herrschaft in sich selbst.</t>
   </si>
   <si>
-    <t>survival-best</t>
+    <t>survival_best</t>
   </si>
   <si>
     <t>Im Unternehmen setzt sich der oder die Beste durch.</t>
@@ -253,7 +253,7 @@
     <t>In the office, whoever is best, succeeds.</t>
   </si>
   <si>
-    <t>whole-person</t>
+    <t>whole_person</t>
   </si>
   <si>
     <t>In meinem Job werde ich als ganze Person anerkannt.</t>
@@ -268,7 +268,7 @@
     <t>Subjektivierung des Arbeitnehmers</t>
   </si>
   <si>
-    <t>stay-til-retirement</t>
+    <t>stay_til_retirement</t>
   </si>
   <si>
     <t>In meinen jetztigem Unternehmen würde ich auch bis zur Rente bleiben.</t>
@@ -280,7 +280,7 @@
     <t>I’d be happy to stay in my current job until retirement.</t>
   </si>
   <si>
-    <t>decide-teammates</t>
+    <t>decide_teammates</t>
   </si>
   <si>
     <t>In meiner Arbeit bestimme ich selbst, mit wem ich eng zusammenarbeite.</t>
@@ -292,7 +292,7 @@
     <t>In my work, I decide with whom I work together.</t>
   </si>
   <si>
-    <t>coop-comp</t>
+    <t>coop_comp</t>
   </si>
   <si>
     <t>In meiner Arbeit bringt einen Kooperation weiter als Wettbewerb.</t>
@@ -304,7 +304,7 @@
     <t>In my line of work, cooperation gets you farther than competition.</t>
   </si>
   <si>
-    <t>goal-not-means</t>
+    <t>goal_not_means</t>
   </si>
   <si>
     <t>In meiner Arbeit ist mir das Ziel vorgegeben, aber nicht der Weg.</t>
@@ -319,7 +319,7 @@
     <t>Handlungsspielräume + Gestaltung</t>
   </si>
   <si>
-    <t>emot-aspects-matter</t>
+    <t>emot_aspects_matter</t>
   </si>
   <si>
     <t>In meiner Arbeit sind Teamfähigkeit, emotionale Intelligenz und Empathie wichtig.</t>
@@ -334,7 +334,7 @@
     <t>Subjektivierung des Unternehmens</t>
   </si>
   <si>
-    <t>recognition-pay</t>
+    <t>recognition_pay</t>
   </si>
   <si>
     <t>Indem ich anständig bezahlt werde, fühle ich mich im Unternehmen geschätzt.</t>
@@ -349,7 +349,7 @@
     <t>Anerkennung (Bezahlung)</t>
   </si>
   <si>
-    <t>clear-guidelines</t>
+    <t>clear_guidelines</t>
   </si>
   <si>
     <t>Klare Vorgaben machen meine Arbeit leichter.</t>
@@ -361,7 +361,7 @@
     <t>Clear guidelines make my work much easier.</t>
   </si>
   <si>
-    <t>same-rope</t>
+    <t>same_rope</t>
   </si>
   <si>
     <t>Letztlich ziehen Arbeitnehmer und Arbeitgeber an einem Strang.</t>
@@ -373,7 +373,7 @@
     <t>At the end of the day, employee and employer are tugging at the same rope.</t>
   </si>
   <si>
-    <t>no-tenure-flexible</t>
+    <t>no_tenure_flexible</t>
   </si>
   <si>
     <t>Mein Arbeitsverhältnis ist befristet, so bleibe ich flexibel.</t>
@@ -385,7 +385,7 @@
     <t>I do not have tenure at my job, but that keeps me flexible.</t>
   </si>
   <si>
-    <t>exchange-value</t>
+    <t>exchange_value</t>
   </si>
   <si>
     <t>Meine Arbeit ist wert, was andere dafür bereit sind zu zahlen.</t>
@@ -397,7 +397,7 @@
     <t>The worth of my work is determined by what others are willing to pay for it.</t>
   </si>
   <si>
-    <t>use-value</t>
+    <t>use_value</t>
   </si>
   <si>
     <t>Meine Arbeit ist wert, was sie anderen nutzt.</t>
@@ -409,7 +409,7 @@
     <t>The worth of my work is determined by how useful it is to others.</t>
   </si>
   <si>
-    <t>friends-family</t>
+    <t>friends_family</t>
   </si>
   <si>
     <t>Meine Freizeit widme ich meinen Freunden und meinen Hobbies.</t>
@@ -424,7 +424,7 @@
     <t>https://medium.com/desk-of-van-schneider/work-life-balance-is-bullshit-f51bf8b3767#.k0k9tmdww</t>
   </si>
   <si>
-    <t>free-free-time</t>
+    <t>free_free_time</t>
   </si>
   <si>
     <t>Meine Freizeit will ich nicht auch noch verplanen.</t>
@@ -436,7 +436,7 @@
     <t>I do not want to have my free time to be all planned.</t>
   </si>
   <si>
-    <t>own-interests</t>
+    <t>own_interests</t>
   </si>
   <si>
     <t>Meine Interessen als Arbeitnehmer setze ich alleine durch.</t>
@@ -451,7 +451,7 @@
     <t>Arbeit jenseits von Interessenskonflikten?</t>
   </si>
   <si>
-    <t>hard-structuring</t>
+    <t>hard_structuring</t>
   </si>
   <si>
     <t>Mir fällt es schwer, meinen Arbeitstag selbständig zu strukturieren.</t>
@@ -463,7 +463,7 @@
     <t>I have a hard time structuring my work day.</t>
   </si>
   <si>
-    <t>full-part-time-dec</t>
+    <t>full_part_time_dec</t>
   </si>
   <si>
     <t>Ob ich Vollzeit oder Teilzeit arbeite, bestimme ich nach meinen Interessen.</t>
@@ -478,7 +478,7 @@
     <t>Vollzeit/Teilzeit</t>
   </si>
   <si>
-    <t>overwhelmed-work</t>
+    <t>overwhelmed_work</t>
   </si>
   <si>
     <t>Oft habe ich das Gefühl, ich schaffe meine Arbeit nicht.</t>
@@ -490,7 +490,7 @@
     <t>I often feel overwhelmed by all my work.</t>
   </si>
   <si>
-    <t>support-weaker</t>
+    <t>support_weaker</t>
   </si>
   <si>
     <t>Schwächere Kollegen bin ich auch bereit mitzutragen.</t>
@@ -502,7 +502,7 @@
     <t>I am ready to support weaker co-workers.</t>
   </si>
   <si>
-    <t>make-concessions</t>
+    <t>make_concessions</t>
   </si>
   <si>
     <t>Um die Wettbewerbsfähigkeit meines Unternehmens zu sichern, bin ich auch zu persönlichen Abstrichen bereit.</t>
@@ -523,7 +523,7 @@
     <t>To keep up at work, I make sure to stay physically fit.</t>
   </si>
   <si>
-    <t>on-street</t>
+    <t>on_street</t>
   </si>
   <si>
     <t>Wenn die Geschäfte mal schlechter laufen, lande ich nicht gleich auf der Straße.</t>
@@ -535,7 +535,7 @@
     <t>Even if business takes a downturn, I won’t end up on the street immediately.</t>
   </si>
   <si>
-    <t>passion-long-hours</t>
+    <t>passion_long_hours</t>
   </si>
   <si>
     <t>Wenn man mit Leidenschaft bei der Sache ist, machen einem auch längere Arbeitszeiten nichts aus.</t>
@@ -547,7 +547,7 @@
     <t>If you’re passionate about your work, the long hours don’t matter.</t>
   </si>
   <si>
-    <t>burden-others</t>
+    <t>burden_others</t>
   </si>
   <si>
     <t>Wer nicht 100 Prozent geben kann, gehört nicht in den Job und wird zur Belastung für andere.</t>
@@ -559,7 +559,7 @@
     <t>If you can’t give 100 percent, you don’t belong and you’re a burden to others.</t>
   </si>
   <si>
-    <t>responsibility-stress</t>
+    <t>responsibility_stress</t>
   </si>
   <si>
     <t>Zu viel Eigenverantwortung stresst mich.</t>
@@ -604,7 +604,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -619,16 +619,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -645,16 +645,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -677,8 +677,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -816,13 +816,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -921,10 +915,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1179,13 +1173,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1498,10 +1486,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>